<commit_message>
Found modes/means for gridblocks - Ensemble
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/Comparing_Model_Runs - With RatioTests.xlsx
+++ b/Excel & CSV Sheets/Comparing_Model_Runs - With RatioTests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Comparing Model Runs" sheetId="1" state="visible" r:id="rId2"/>
@@ -5224,7 +5224,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7450,7 +7450,7 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -10925,8 +10925,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>